<commit_message>
Draft 1 for advisor
Final changes for draft to advisor
</commit_message>
<xml_diff>
--- a/data/raw-data/Mean_Birthweights.xlsx
+++ b/data/raw-data/Mean_Birthweights.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassiaroth/Documents/GitHub/MADARoth/Roth-MADA-project/data/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassiaroth/Documents/GitHub/MADARoth/Roth-ML-project/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64342AFE-35B3-934E-8D92-7A3B0A281C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07975EDA-8208-BA44-96F7-F5E86C542CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="10560" windowWidth="27640" windowHeight="16940" xr2:uid="{02D297A7-6752-E444-A718-DAC613517E94}"/>
+    <workbookView xWindow="20340" yWindow="8720" windowWidth="27640" windowHeight="16940" xr2:uid="{02D297A7-6752-E444-A718-DAC613517E94}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Calculations" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Sample</t>
   </si>
@@ -49,160 +50,169 @@
     <t>Median</t>
   </si>
   <si>
-    <t>&lt;=2500gm (percentage)</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>Boston New England</t>
-  </si>
-  <si>
     <t>1872-1900</t>
   </si>
   <si>
-    <t>Boston Lying-In (Indoors)</t>
-  </si>
-  <si>
     <t>1886-1900</t>
   </si>
   <si>
-    <t>Boston Lying-In (Outdoors)</t>
-  </si>
-  <si>
     <t>1884-1900</t>
   </si>
   <si>
-    <t>New York Lying-In (singeltons)</t>
-  </si>
-  <si>
-    <t>1910-1931</t>
-  </si>
-  <si>
     <t>Maternal Age (mean)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ward, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Birth Weight</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, p. 148-9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Costa, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Unequal at Birth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, p. 991-2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Costa, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Race and Pregnancy</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, p. 1065</t>
-    </r>
-  </si>
-  <si>
     <t>1897-1935</t>
   </si>
   <si>
-    <t>Johns Hopkins (singletons - white)</t>
-  </si>
-  <si>
-    <t>Johns Hopkins (singletons - Black)</t>
-  </si>
-  <si>
-    <t>Antebellum U.S. South</t>
-  </si>
-  <si>
-    <t>Steckel, 1986, p. 174, 182</t>
-  </si>
-  <si>
-    <t>1848-1873</t>
-  </si>
-  <si>
-    <t>Philadelphia Almshouse (all births)</t>
-  </si>
-  <si>
-    <t>Philadelphia Almshouse (live births)</t>
-  </si>
-  <si>
     <t>&lt;1850</t>
   </si>
   <si>
-    <t>Goldin, 1989, p. 363-5</t>
-  </si>
-  <si>
-    <t>1907-1922</t>
-  </si>
-  <si>
-    <t>St. Helens Hospital, Wellington, New Zealand (singleton live births)</t>
-  </si>
-  <si>
-    <t>St. Helens Hospital, Wellington, New Zealand (singleton live female births)</t>
-  </si>
-  <si>
-    <t>St. Helens Hospital, Wellington, New Zealand (singleton live male births)</t>
-  </si>
-  <si>
-    <t>Roberts and Wood, 156, 158</t>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Baltimore (white singletons)</t>
+  </si>
+  <si>
+    <t>Philadelphia (live)</t>
+  </si>
+  <si>
+    <t>Philadelphia (all)</t>
+  </si>
+  <si>
+    <t>Boston (in hospital)</t>
+  </si>
+  <si>
+    <t>Boston (at home)</t>
+  </si>
+  <si>
+    <t>New York (singeltons)</t>
+  </si>
+  <si>
+    <t>Baltimore (Black singletons)</t>
+  </si>
+  <si>
+    <t>1999-2001</t>
+  </si>
+  <si>
+    <t>Riberão Preto, São Paulo, Brazil</t>
+  </si>
+  <si>
+    <t>Pelotas, Rio Grande do Sul, Brazil (live singletons)</t>
+  </si>
+  <si>
+    <t>1848-73</t>
+  </si>
+  <si>
+    <t>1907-22</t>
+  </si>
+  <si>
+    <t>1910-31</t>
+  </si>
+  <si>
+    <t>1922-26</t>
+  </si>
+  <si>
+    <t>Maternidade Laranjeiras</t>
+  </si>
+  <si>
+    <t>1978-79</t>
+  </si>
+  <si>
+    <t>1993-98</t>
+  </si>
+  <si>
+    <t>&lt;2500gm (%)</t>
+  </si>
+  <si>
+    <t>Steckel, 1986, 174, 182</t>
+  </si>
+  <si>
+    <t>Goldin, 1989, 363-5</t>
+  </si>
+  <si>
+    <t>Ward, 1993, 148-9</t>
+  </si>
+  <si>
+    <t>Costa, 2004,  1065</t>
+  </si>
+  <si>
+    <t>Costa, 2004, 1065</t>
+  </si>
+  <si>
+    <t>Roberts, 2014, 156, 158</t>
+  </si>
+  <si>
+    <t>Costa, 1998,  991-2</t>
+  </si>
+  <si>
+    <t>Silva, 1998, 77</t>
+  </si>
+  <si>
+    <t>Silveira, 2019, i48</t>
+  </si>
+  <si>
+    <t>Monteiro, 2000, 31</t>
+  </si>
+  <si>
+    <t>Leal, 2006, 469</t>
+  </si>
+  <si>
+    <t>Leal, 2006, 470</t>
+  </si>
+  <si>
+    <t>Antebellum US South (estimated enslaved)</t>
+  </si>
+  <si>
+    <t>Wellington, NZ (singleton live)</t>
+  </si>
+  <si>
+    <t>Wellington, NZ (singleton live female)</t>
+  </si>
+  <si>
+    <t>Wellington, NZ (singleton live male)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (White singletons, mothers incomplete K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (singletons all)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (White singletons)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Mixed-race singletons)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Black singletons)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (female singletons)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (male singletons)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Mixed-race singletons, mothers incomplete K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Black singletons, mothers incomplete K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (White singletons, mothers complete K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Mixed-race singletons, mothers complete K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Black singletons, mothers complete K-12)</t>
+  </si>
+  <si>
+    <t>São Paulo, Brazil (live)</t>
   </si>
 </sst>
 </file>
@@ -226,15 +236,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,10 +274,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,15 +592,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FDFB52-F3CB-7842-BE7C-C46CE0D1BF2F}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
@@ -611,237 +620,599 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="3">
+        <v>10</v>
+      </c>
+      <c r="C2">
         <v>2320</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>3403</v>
-      </c>
-      <c r="D3">
-        <v>3461</v>
-      </c>
-      <c r="E3">
-        <v>8.1</v>
+      <c r="C3" s="3">
+        <v>3037</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>3375</v>
-      </c>
-      <c r="D4">
-        <v>3453</v>
-      </c>
-      <c r="E4">
-        <v>9.6</v>
+        <v>25</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3038</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>3480</v>
-      </c>
-      <c r="E5">
-        <v>6.5</v>
+        <v>25</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3064</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>3330</v>
-      </c>
-      <c r="E6">
-        <v>6.9</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3087</v>
+      </c>
+      <c r="F6">
+        <v>25.3</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7">
-        <v>3479</v>
-      </c>
-      <c r="E7">
-        <v>4.7</v>
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>1994</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3115</v>
+      </c>
+      <c r="D7">
+        <v>3150</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8">
-        <v>3463</v>
-      </c>
-      <c r="D8">
-        <v>3467</v>
-      </c>
-      <c r="E8">
-        <v>5.5</v>
-      </c>
-      <c r="F8">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3122</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9">
-        <v>3423</v>
-      </c>
-      <c r="D9">
-        <v>3443</v>
-      </c>
-      <c r="E9">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3133</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10">
-        <v>3183</v>
-      </c>
-      <c r="D10">
-        <v>3175</v>
-      </c>
-      <c r="E10">
-        <v>11.4</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3137</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11">
-        <v>3467</v>
-      </c>
-      <c r="E11">
-        <v>4.2</v>
-      </c>
-      <c r="F11">
-        <v>27.75</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3154</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="C12">
-        <v>3403</v>
+      <c r="C12" s="3">
+        <v>3155</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>2004</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3167</v>
+      </c>
+      <c r="E13">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1993</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3169</v>
+      </c>
+      <c r="E14">
+        <v>9.1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>3183</v>
+      </c>
+      <c r="D15">
+        <v>3175</v>
+      </c>
+      <c r="E15">
+        <v>11.4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3">
+        <v>3185</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3">
+        <v>3186</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>2015</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3198</v>
+      </c>
+      <c r="E18">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1982</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3201</v>
+      </c>
+      <c r="E19">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3210</v>
+      </c>
+      <c r="G20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3">
+        <v>3218</v>
+      </c>
+      <c r="G21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3234</v>
+      </c>
+      <c r="D22">
+        <v>3250</v>
+      </c>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>3330</v>
+      </c>
+      <c r="E23">
+        <v>6.9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>3375</v>
+      </c>
+      <c r="D24">
+        <v>3453</v>
+      </c>
+      <c r="E24">
+        <v>9.6</v>
+      </c>
+      <c r="G24" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>3403</v>
+      </c>
+      <c r="D25">
+        <v>3461</v>
+      </c>
+      <c r="E25">
+        <v>8.1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>3403</v>
+      </c>
+      <c r="G26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>3423</v>
+      </c>
+      <c r="D27">
+        <v>3443</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>3463</v>
+      </c>
+      <c r="D28">
+        <v>3467</v>
+      </c>
+      <c r="E28">
+        <v>5.5</v>
+      </c>
+      <c r="F28">
+        <v>27</v>
+      </c>
+      <c r="G28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29">
+        <v>3467</v>
+      </c>
+      <c r="E29">
+        <v>4.2</v>
+      </c>
+      <c r="F29">
+        <v>27.75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>3479</v>
+      </c>
+      <c r="E30">
+        <v>4.7</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>3480</v>
+      </c>
+      <c r="E31">
+        <v>6.5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32">
         <v>3531</v>
       </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E20">
-        <f>5.8+2.1+1.2+0.5</f>
-        <v>9.6</v>
-      </c>
-      <c r="F20">
-        <f>0.3+0.8+1.7+5.3</f>
-        <v>8.1</v>
+      <c r="G32" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">
+    <sortCondition ref="C2:C32"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453B3B05-433E-CE48-B901-3BDD40D65F8B}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>3142</v>
+      </c>
+      <c r="B1">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3139</v>
+      </c>
+      <c r="B2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3153</v>
+      </c>
+      <c r="B3">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3167</v>
+      </c>
+      <c r="B4">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3166</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3161</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>SUM(A1:A6)/6</f>
+        <v>3154.6666666666665</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B1:B6)/6</f>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revisions for submission 2
After call w/Bill
</commit_message>
<xml_diff>
--- a/data/raw-data/Mean_Birthweights.xlsx
+++ b/data/raw-data/Mean_Birthweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10804"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassiaroth/Documents/GitHub/MADARoth/Roth-ML-project/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07975EDA-8208-BA44-96F7-F5E86C542CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E194D18-688B-4B4D-9FA7-D86AD7D28D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20340" yWindow="8720" windowWidth="27640" windowHeight="16940" xr2:uid="{02D297A7-6752-E444-A718-DAC613517E94}"/>
+    <workbookView xWindow="6220" yWindow="9920" windowWidth="27640" windowHeight="16940" xr2:uid="{02D297A7-6752-E444-A718-DAC613517E94}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
   <si>
     <t>Sample</t>
   </si>
@@ -116,9 +116,6 @@
     <t>1922-26</t>
   </si>
   <si>
-    <t>Maternidade Laranjeiras</t>
-  </si>
-  <si>
     <t>1978-79</t>
   </si>
   <si>
@@ -128,42 +125,6 @@
     <t>&lt;2500gm (%)</t>
   </si>
   <si>
-    <t>Steckel, 1986, 174, 182</t>
-  </si>
-  <si>
-    <t>Goldin, 1989, 363-5</t>
-  </si>
-  <si>
-    <t>Ward, 1993, 148-9</t>
-  </si>
-  <si>
-    <t>Costa, 2004,  1065</t>
-  </si>
-  <si>
-    <t>Costa, 2004, 1065</t>
-  </si>
-  <si>
-    <t>Roberts, 2014, 156, 158</t>
-  </si>
-  <si>
-    <t>Costa, 1998,  991-2</t>
-  </si>
-  <si>
-    <t>Silva, 1998, 77</t>
-  </si>
-  <si>
-    <t>Silveira, 2019, i48</t>
-  </si>
-  <si>
-    <t>Monteiro, 2000, 31</t>
-  </si>
-  <si>
-    <t>Leal, 2006, 469</t>
-  </si>
-  <si>
-    <t>Leal, 2006, 470</t>
-  </si>
-  <si>
     <t>Antebellum US South (estimated enslaved)</t>
   </si>
   <si>
@@ -176,9 +137,6 @@
     <t>Wellington, NZ (singleton live male)</t>
   </si>
   <si>
-    <t>Rio de Janeiro (White singletons, mothers incomplete K-12)</t>
-  </si>
-  <si>
     <t>Rio de Janeiro (singletons all)</t>
   </si>
   <si>
@@ -197,22 +155,79 @@
     <t>Rio de Janeiro (male singletons)</t>
   </si>
   <si>
-    <t>Rio de Janeiro (Mixed-race singletons, mothers incomplete K-12)</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro (Black singletons, mothers incomplete K-12)</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro (White singletons, mothers complete K-12)</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro (Mixed-race singletons, mothers complete K-12)</t>
-  </si>
-  <si>
-    <t>Rio de Janeiro (Black singletons, mothers complete K-12)</t>
-  </si>
-  <si>
     <t>São Paulo, Brazil (live)</t>
+  </si>
+  <si>
+    <t>Laranjeiras</t>
+  </si>
+  <si>
+    <t>Steckel, 1986</t>
+  </si>
+  <si>
+    <t>Page #</t>
+  </si>
+  <si>
+    <t>174, 182</t>
+  </si>
+  <si>
+    <t>Silva, 1998</t>
+  </si>
+  <si>
+    <t>Leal, 2006</t>
+  </si>
+  <si>
+    <t>i48</t>
+  </si>
+  <si>
+    <t>148-9</t>
+  </si>
+  <si>
+    <t>Monteiro, 2000</t>
+  </si>
+  <si>
+    <t>Silveira, 2019</t>
+  </si>
+  <si>
+    <t>Costa, 2004</t>
+  </si>
+  <si>
+    <t>Ward, 1993</t>
+  </si>
+  <si>
+    <t>363-5</t>
+  </si>
+  <si>
+    <t>156, 158</t>
+  </si>
+  <si>
+    <t>991-2</t>
+  </si>
+  <si>
+    <t>Goldin, 1989</t>
+  </si>
+  <si>
+    <t>Roberts, 2014</t>
+  </si>
+  <si>
+    <t>Costa, 1998</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Black singletons, mothers &lt;K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Mixed-race singletons, mothers &lt;K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (White singletons, mothers &lt;K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Black singletons, mothers  &gt;=K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Mixed-race singletons, mothers &gt;=K-12)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (White singletons, mothers &gt;=K-12)</t>
   </si>
 </sst>
 </file>
@@ -296,9 +311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -336,7 +351,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -442,7 +457,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -584,7 +599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -592,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FDFB52-F3CB-7842-BE7C-C46CE0D1BF2F}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,7 +621,7 @@
     <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -628,10 +643,13 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -640,12 +658,15 @@
         <v>2320</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -654,12 +675,12 @@
         <v>3037</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
@@ -668,12 +689,12 @@
         <v>3038</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -682,12 +703,12 @@
         <v>3064</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -699,10 +720,10 @@
         <v>25.3</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -716,12 +737,15 @@
         <v>3150</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="H7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -730,12 +754,15 @@
         <v>3122</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -744,12 +771,12 @@
         <v>3133</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -758,12 +785,12 @@
         <v>3137</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -772,15 +799,18 @@
         <v>3154</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H11">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="3">
         <v>3155</v>
@@ -789,10 +819,13 @@
         <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="H12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -806,10 +839,13 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -823,10 +859,13 @@
         <v>9.1</v>
       </c>
       <c r="G14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -843,12 +882,15 @@
         <v>11.4</v>
       </c>
       <c r="G15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
@@ -857,12 +899,15 @@
         <v>3185</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H16">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
@@ -871,10 +916,13 @@
         <v>3186</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H17">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -888,10 +936,13 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -905,12 +956,15 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -919,12 +973,15 @@
         <v>3210</v>
       </c>
       <c r="G20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H20">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -933,15 +990,18 @@
         <v>3218</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="H21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3">
         <v>3234</v>
@@ -950,10 +1010,13 @@
         <v>3250</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="H22">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -967,10 +1030,13 @@
         <v>6.9</v>
       </c>
       <c r="G23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="H23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -987,10 +1053,13 @@
         <v>9.6</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="H24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1007,12 +1076,15 @@
         <v>8.1</v>
       </c>
       <c r="G25" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>44</v>
       </c>
       <c r="B26" t="s">
         <v>23</v>
@@ -1021,10 +1093,13 @@
         <v>3403</v>
       </c>
       <c r="G26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="H26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1041,10 +1116,13 @@
         <v>6</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1064,12 +1142,15 @@
         <v>27</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="H28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -1084,10 +1165,13 @@
         <v>27.75</v>
       </c>
       <c r="G29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="H29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1101,10 +1185,13 @@
         <v>4.7</v>
       </c>
       <c r="G30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1118,12 +1205,15 @@
         <v>6.5</v>
       </c>
       <c r="G31" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>45</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
@@ -1132,7 +1222,10 @@
         <v>3531</v>
       </c>
       <c r="G32" t="s">
-        <v>35</v>
+        <v>56</v>
+      </c>
+      <c r="H32" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final Changes for RR
Created DiB; updates for all changes
</commit_message>
<xml_diff>
--- a/data/raw-data/Mean_Birthweights.xlsx
+++ b/data/raw-data/Mean_Birthweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10804"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cassiaroth/Documents/GitHub/MADARoth/Roth-ML-project/data/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E194D18-688B-4B4D-9FA7-D86AD7D28D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69093DB6-173E-AD41-BB1E-8CD9EF478F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6220" yWindow="9920" windowWidth="27640" windowHeight="16940" xr2:uid="{02D297A7-6752-E444-A718-DAC613517E94}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="31420" windowHeight="27080" xr2:uid="{02D297A7-6752-E444-A718-DAC613517E94}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="71">
   <si>
     <t>Sample</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Boston (at home)</t>
   </si>
   <si>
-    <t>New York (singeltons)</t>
-  </si>
-  <si>
     <t>Baltimore (Black singletons)</t>
   </si>
   <si>
@@ -221,13 +218,37 @@
     <t>Rio de Janeiro (White singletons, mothers &lt;K-12)</t>
   </si>
   <si>
-    <t>Rio de Janeiro (Black singletons, mothers  &gt;=K-12)</t>
-  </si>
-  <si>
     <t>Rio de Janeiro (Mixed-race singletons, mothers &gt;=K-12)</t>
   </si>
   <si>
     <t>Rio de Janeiro (White singletons, mothers &gt;=K-12)</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>mean and median</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>156, 158, 159</t>
+  </si>
+  <si>
+    <t>156, 157, 158</t>
+  </si>
+  <si>
+    <t>Boston (Black)</t>
+  </si>
+  <si>
+    <t>estimated coefficient</t>
+  </si>
+  <si>
+    <t>New York (singletons)</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro (Black singletons, mothers &gt;=K-12)</t>
   </si>
 </sst>
 </file>
@@ -607,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FDFB52-F3CB-7842-BE7C-C46CE0D1BF2F}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,7 +642,7 @@
     <col min="7" max="7" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +656,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -644,12 +665,15 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -658,60 +682,72 @@
         <v>2320</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3">
         <v>3037</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3">
         <v>3038</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3">
         <v>3064</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="3">
         <v>3087</v>
@@ -720,12 +756,15 @@
         <v>25.3</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>1994</v>
@@ -737,432 +776,492 @@
         <v>3150</v>
       </c>
       <c r="G7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3">
         <v>3122</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H8">
         <v>469</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>3126</v>
+      </c>
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9">
+        <v>149</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3">
         <v>3133</v>
       </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3137</v>
+      </c>
+      <c r="G11" t="s">
+        <v>39</v>
+      </c>
+      <c r="I11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3154</v>
+      </c>
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12">
+        <v>469</v>
+      </c>
+      <c r="I12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3137</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3">
-        <v>3154</v>
-      </c>
-      <c r="G11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="3">
         <v>3155</v>
-      </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13">
-        <v>2004</v>
-      </c>
-      <c r="C13" s="3">
-        <v>3167</v>
       </c>
       <c r="E13">
         <v>9</v>
       </c>
       <c r="G13" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13">
+        <v>31</v>
+      </c>
+      <c r="I13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>2004</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3167</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>1993</v>
+      </c>
+      <c r="C15" s="3">
+        <v>3169</v>
+      </c>
+      <c r="E15">
+        <v>9.1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>3183</v>
+      </c>
+      <c r="D16">
+        <v>3175</v>
+      </c>
+      <c r="E16">
+        <v>11.4</v>
+      </c>
+      <c r="G16" t="s">
         <v>49</v>
       </c>
-      <c r="H13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>1993</v>
-      </c>
-      <c r="C14" s="3">
-        <v>3169</v>
-      </c>
-      <c r="E14">
-        <v>9.1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="H16">
+        <v>1065</v>
+      </c>
+      <c r="I16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15">
-        <v>3183</v>
-      </c>
-      <c r="D15">
-        <v>3175</v>
-      </c>
-      <c r="E15">
-        <v>11.4</v>
-      </c>
-      <c r="G15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="C17" s="3">
         <v>3185</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17">
+        <v>470</v>
+      </c>
+      <c r="I17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3186</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18">
+        <v>469</v>
+      </c>
+      <c r="I18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>2015</v>
+      </c>
+      <c r="C19" s="3">
+        <v>3198</v>
+      </c>
+      <c r="E19">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G19" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" t="s">
         <v>45</v>
       </c>
-      <c r="H16">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1982</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3201</v>
+      </c>
+      <c r="E20">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G20" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="3">
-        <v>3186</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18">
-        <v>2015</v>
-      </c>
-      <c r="C18" s="3">
-        <v>3198</v>
-      </c>
-      <c r="E18">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="G18" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19">
-        <v>1982</v>
-      </c>
-      <c r="C19" s="3">
-        <v>3201</v>
-      </c>
-      <c r="E19">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="G19" t="s">
-        <v>49</v>
-      </c>
-      <c r="H19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="3">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
         <v>3210</v>
       </c>
-      <c r="G20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="3">
-        <v>3218</v>
-      </c>
       <c r="G21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H21">
         <v>470</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C22" s="3">
-        <v>3234</v>
-      </c>
-      <c r="D22">
-        <v>3250</v>
+        <v>3218</v>
       </c>
       <c r="G22" t="s">
         <v>44</v>
       </c>
       <c r="H22">
+        <v>470</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3">
+        <v>3234</v>
+      </c>
+      <c r="D23">
+        <v>3250</v>
+      </c>
+      <c r="G23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="I23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>15</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>3330</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>6.9</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>3375</v>
+      </c>
+      <c r="D25">
+        <v>3453</v>
+      </c>
+      <c r="E25">
+        <v>9.6</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="s">
         <v>51</v>
       </c>
-      <c r="H23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24">
-        <v>3375</v>
-      </c>
-      <c r="D24">
-        <v>3453</v>
-      </c>
-      <c r="E24">
-        <v>9.6</v>
-      </c>
-      <c r="G24" t="s">
-        <v>55</v>
-      </c>
-      <c r="H24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="I25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>13</v>
       </c>
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25">
-        <v>3403</v>
-      </c>
-      <c r="D25">
-        <v>3461</v>
-      </c>
-      <c r="E25">
-        <v>8.1</v>
-      </c>
-      <c r="G25" t="s">
-        <v>55</v>
-      </c>
-      <c r="H25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>3403</v>
       </c>
+      <c r="D26">
+        <v>3461</v>
+      </c>
+      <c r="E26">
+        <v>8.1</v>
+      </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="I26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>3403</v>
+      </c>
+      <c r="G27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s">
+        <v>52</v>
+      </c>
+      <c r="I27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>12</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>9</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>3423</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>3443</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <v>6</v>
       </c>
-      <c r="G27" t="s">
-        <v>50</v>
-      </c>
-      <c r="H27">
+      <c r="G28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H28">
         <v>1065</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28">
-        <v>3463</v>
-      </c>
-      <c r="D28">
-        <v>3467</v>
-      </c>
-      <c r="E28">
-        <v>5.5</v>
-      </c>
-      <c r="F28">
-        <v>27</v>
-      </c>
-      <c r="G28" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
       </c>
       <c r="C29">
+        <v>3463</v>
+      </c>
+      <c r="D29">
         <v>3467</v>
       </c>
       <c r="E29">
-        <v>4.2</v>
+        <v>5.5</v>
       </c>
       <c r="F29">
-        <v>27.75</v>
+        <v>27</v>
       </c>
       <c r="G29" t="s">
         <v>56</v>
@@ -1170,67 +1269,108 @@
       <c r="H29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>3467</v>
+      </c>
+      <c r="E30">
+        <v>4.2</v>
+      </c>
+      <c r="F30">
+        <v>27.75</v>
+      </c>
+      <c r="G30" t="s">
+        <v>55</v>
+      </c>
+      <c r="H30" t="s">
+        <v>66</v>
+      </c>
+      <c r="I30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>16</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>7</v>
       </c>
-      <c r="C30">
+      <c r="C31">
         <v>3479</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>4.7</v>
       </c>
-      <c r="G30" t="s">
-        <v>51</v>
-      </c>
-      <c r="H30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="G31" t="s">
+        <v>50</v>
+      </c>
+      <c r="H31" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C31">
+      <c r="C32">
         <v>3480</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <v>6.5</v>
       </c>
-      <c r="G31" t="s">
-        <v>51</v>
-      </c>
-      <c r="H31" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32">
+      <c r="G32" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33">
         <v>3531</v>
       </c>
-      <c r="G32" t="s">
-        <v>56</v>
-      </c>
-      <c r="H32" t="s">
-        <v>53</v>
+      <c r="D33">
+        <v>3574</v>
+      </c>
+      <c r="G33" t="s">
+        <v>55</v>
+      </c>
+      <c r="H33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I33" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G32">
-    <sortCondition ref="C2:C32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J33">
+    <sortCondition ref="C2:C33"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>